<commit_message>
Documents: Updated validation guide to latest V&V results
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="4260" windowWidth="25600" windowHeight="18760" tabRatio="500"/>
+    <workbookView xWindow="8955" yWindow="4260" windowWidth="25605" windowHeight="18765" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -81,7 +81,7 @@
     <t>2 sigma M</t>
   </si>
   <si>
-    <t>RP all</t>
+    <t>RP all (with new LLNL comparisons)</t>
   </si>
 </sst>
 </file>
@@ -243,6 +243,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -571,15 +576,15 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +609,7 @@
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -638,7 +643,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -663,10 +668,10 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.27</v>
       </c>
       <c r="K3" s="3">
-        <v>0.44</v>
+        <v>0.59</v>
       </c>
       <c r="L3" s="3">
         <v>7.0000000000000007E-2</v>
@@ -676,7 +681,7 @@
       <c r="P3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -714,7 +719,7 @@
       <c r="P4" s="3"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -752,7 +757,7 @@
       <c r="P5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -792,7 +797,7 @@
       <c r="P6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -812,7 +817,7 @@
       <c r="P7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -850,7 +855,7 @@
       <c r="P8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -882,7 +887,7 @@
       <c r="P9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -912,7 +917,7 @@
       <c r="P10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -942,7 +947,7 @@
       <c r="P11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -980,7 +985,7 @@
       <c r="P12" s="3"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1018,7 +1023,7 @@
       <c r="P13" s="5"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1049,7 @@
       <c r="P14" s="6"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1083,7 +1088,7 @@
       <c r="P15" s="3"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>

</xml_diff>

<commit_message>
cfast source: updated input.f to fortran 90.  No change in results verified with full validation suite
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="4260" windowWidth="25605" windowHeight="18765" tabRatio="500"/>
+    <workbookView xWindow="8960" yWindow="4260" windowWidth="25600" windowHeight="18760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Output Quantity</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>RP all (with new LLNL comparisons)</t>
+  </si>
+  <si>
+    <t>LLNL Only</t>
+  </si>
+  <si>
+    <t>All Others</t>
   </si>
 </sst>
 </file>
@@ -137,7 +143,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -171,8 +177,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +209,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -206,7 +219,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -223,6 +236,8 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -239,6 +254,8 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,43 +590,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="4" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -643,7 +660,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -668,203 +685,198 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3">
-        <v>1.27</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K3" s="3">
-        <v>0.59</v>
+        <v>0.47</v>
       </c>
       <c r="L3" s="3">
         <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
       </c>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1.04</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="D4" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
+    <row r="4" spans="1:18">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="3">
-        <v>1.07</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="H4" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3">
-        <v>1.07</v>
+        <v>1.43</v>
       </c>
       <c r="K4" s="3">
-        <v>0.36</v>
-      </c>
-      <c r="L4" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.53</v>
+      </c>
+      <c r="L4" s="3"/>
+      <c r="M4" t="s">
+        <v>21</v>
       </c>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.04</v>
       </c>
       <c r="C5" s="3">
-        <v>0.24</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D5" s="3">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.07</v>
       </c>
       <c r="G5" s="3">
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="H5" s="3">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3">
-        <v>1.31</v>
+        <v>1.07</v>
       </c>
       <c r="K5" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.36</v>
       </c>
       <c r="L5" s="3">
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>1.25</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C6" s="3">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="D6" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <v>1.31</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="G6" s="3">
-        <f>0.27/2</f>
-        <v>0.13500000000000001</v>
+        <v>0.23</v>
       </c>
       <c r="H6" s="3">
-        <f>0.07</f>
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.31</v>
       </c>
       <c r="K6" s="3">
-        <v>0.44</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L6" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="D7" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="F7" s="3">
+        <v>1.31</v>
+      </c>
+      <c r="G7" s="3">
+        <f>0.27/2</f>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="H7" s="3">
+        <f>0.07</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="J7" s="3">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.44</v>
+      </c>
+      <c r="L7" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.91</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.05</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3">
-        <v>1.06</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.05</v>
-      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3">
-        <v>1.06</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0.68</v>
-      </c>
-      <c r="L8" s="3">
-        <v>0.05</v>
-      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.05</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3">
-        <v>0.89</v>
+        <v>1.06</v>
       </c>
       <c r="G9" s="3">
         <v>0.22</v>
@@ -874,10 +886,10 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3">
-        <v>0.93</v>
+        <v>1.06</v>
       </c>
       <c r="K9" s="3">
-        <v>0.47</v>
+        <v>0.68</v>
       </c>
       <c r="L9" s="3">
         <v>0.05</v>
@@ -887,227 +899,260 @@
       <c r="P9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2.65</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.63</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.17</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="F10" s="3">
+        <v>0.89</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.22</v>
+      </c>
       <c r="H10" s="3">
-        <v>0.17</v>
+        <v>0.05</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="J10" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.48</v>
+      </c>
       <c r="L10" s="3">
-        <v>0.17</v>
+        <v>0.05</v>
       </c>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
-        <v>1.1299999999999999</v>
+        <v>2.65</v>
       </c>
       <c r="C11" s="3">
-        <v>0.37</v>
+        <v>0.63</v>
       </c>
       <c r="D11" s="3">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3">
-        <v>1</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="C12" s="3">
-        <v>0.27</v>
+        <v>0.37</v>
       </c>
       <c r="D12" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="3">
-        <v>1.02</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.32</v>
-      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3">
-        <v>1.02</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0.61</v>
-      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
       <c r="L12" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="H13" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="L13" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B14" s="3">
         <v>1.32</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C14" s="3">
         <v>0.54</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="10">
-        <v>1.21</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0.52</v>
-      </c>
-      <c r="H13" s="10">
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="7">
-        <v>1.21</v>
-      </c>
-      <c r="K13" s="7">
-        <v>1.04</v>
-      </c>
-      <c r="L13" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.81</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.47</v>
       </c>
       <c r="D14" s="3">
         <v>0.1</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="F14" s="11">
+        <v>1.21</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0.52</v>
+      </c>
+      <c r="H14" s="11">
+        <v>0.1</v>
+      </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+      <c r="J14" s="7">
+        <v>1.21</v>
+      </c>
+      <c r="K14" s="7">
+        <v>1.04</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.81</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>1.25</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C16" s="3">
         <v>0.48</v>
       </c>
-      <c r="D15" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3">
+      <c r="D16" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
         <v>1.2</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G16" s="3">
         <f>0.75/2</f>
         <v>0.375</v>
       </c>
-      <c r="H15" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3">
+      <c r="H16" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3">
         <v>1.2</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K16" s="3">
         <v>0.75</v>
       </c>
-      <c r="L15" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="R15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="J1:L1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
cfast source: compared revised CFAST (with door jet fires fixed) to complete validation suite and results are fine.
Updated GUI and CFAST to accept a new fire keyword, GLOBA for global fire parameters lower oxygen limit and gaseous ignition temperature.  Verified things work with CHEMI LO, HIGH, and HIGHLIMO2 example cases.
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="4260" windowWidth="25600" windowHeight="18760" tabRatio="500"/>
+    <workbookView xWindow="8955" yWindow="4260" windowWidth="25605" windowHeight="18765" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -182,7 +182,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -193,12 +193,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -593,40 +587,40 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -660,7 +654,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -701,7 +695,7 @@
       <c r="P3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -725,7 +719,7 @@
       <c r="P4" s="3"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -750,10 +744,10 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3">
-        <v>1.07</v>
+        <v>1.04</v>
       </c>
       <c r="K5" s="3">
-        <v>0.36</v>
+        <v>0.34</v>
       </c>
       <c r="L5" s="3">
         <v>7.0000000000000007E-2</v>
@@ -763,7 +757,7 @@
       <c r="P5" s="3"/>
       <c r="R5" s="3"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -801,7 +795,7 @@
       <c r="P6" s="3"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -841,7 +835,7 @@
       <c r="P7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -861,7 +855,7 @@
       <c r="P8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -899,7 +893,7 @@
       <c r="P9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -931,7 +925,7 @@
       <c r="P10" s="3"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -961,7 +955,7 @@
       <c r="P11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -991,7 +985,7 @@
       <c r="P12" s="3"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1029,7 +1023,7 @@
       <c r="P13" s="3"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1043,23 +1037,23 @@
         <v>0.1</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="11">
+      <c r="F14" s="9">
         <v>1.21</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="9">
         <v>0.52</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="9">
         <v>0.1</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="7">
+      <c r="J14" s="9">
         <v>1.21</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="9">
         <v>1.04</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="9">
         <v>0.1</v>
       </c>
       <c r="N14" s="5"/>
@@ -1067,7 +1061,7 @@
       <c r="P14" s="5"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1081,19 +1075,19 @@
         <v>0.1</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1132,7 +1126,7 @@
       <c r="P16" s="3"/>
       <c r="R16" s="3"/>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -1146,16 +1140,19 @@
       <c r="L17" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Validation: Updated NUREG 1824 validation script and data to match current script format.
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Output Quantity</t>
   </si>
@@ -75,19 +75,10 @@
     <t>NUREG-1934</t>
   </si>
   <si>
-    <t>RP, 1824 only</t>
-  </si>
-  <si>
-    <t>2 sigma M</t>
-  </si>
-  <si>
-    <t>RP all (with new LLNL comparisons)</t>
-  </si>
-  <si>
-    <t>LLNL Only</t>
-  </si>
-  <si>
-    <t>All Others</t>
+    <t>RP, 1824 only (new McT algorithm)</t>
+  </si>
+  <si>
+    <t>RP all  (new McT algorithm)</t>
   </si>
 </sst>
 </file>
@@ -584,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R17"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -595,7 +586,7 @@
     <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -612,15 +603,14 @@
       <c r="H1" s="8"/>
       <c r="I1" s="7"/>
       <c r="J1" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
+      <c r="M1" s="4"/>
       <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -645,16 +635,15 @@
         <v>1</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -669,487 +658,449 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3">
-        <v>1.05</v>
+        <v>0.99</v>
       </c>
       <c r="G3" s="3">
-        <v>0.12</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H3" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="K3" s="3">
-        <v>0.47</v>
+        <v>0.215</v>
       </c>
       <c r="L3" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
+      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D4" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="F4" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H4" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3">
-        <v>1.43</v>
+        <v>1.04</v>
       </c>
       <c r="K4" s="3">
-        <v>0.53</v>
-      </c>
-      <c r="L4" s="3"/>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
+        <v>0.15</v>
+      </c>
+      <c r="L4" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
-        <v>1.04</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C5" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.24</v>
       </c>
       <c r="D5" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
-        <v>1.07</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="G5" s="3">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="H5" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3">
-        <v>1.04</v>
+        <v>1.19</v>
       </c>
       <c r="K5" s="3">
-        <v>0.34</v>
+        <v>0.18</v>
       </c>
       <c r="L5" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="R5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.25</v>
       </c>
       <c r="C6" s="3">
-        <v>0.24</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D6" s="3">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.32</v>
       </c>
       <c r="G6" s="3">
-        <v>0.23</v>
+        <v>0.11</v>
       </c>
       <c r="H6" s="3">
-        <v>0.05</v>
+        <f>0.07</f>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3">
-        <v>1.31</v>
+        <v>1.17</v>
       </c>
       <c r="K6" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.215</v>
       </c>
       <c r="L6" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="D8" s="3">
         <v>0.05</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="R6" s="3"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="D7" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3">
-        <v>1.31</v>
-      </c>
-      <c r="G7" s="3">
-        <f>0.27/2</f>
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="H7" s="3">
-        <f>0.07</f>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="K7" s="3">
-        <v>0.44</v>
-      </c>
-      <c r="L7" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="F8" s="3">
+        <v>1.04</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.05</v>
+      </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="J8" s="3">
+        <v>0.97</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.32</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.91</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.05</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3">
-        <v>1.06</v>
+        <v>0.91</v>
       </c>
       <c r="G9" s="3">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="H9" s="3">
         <v>0.05</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3">
-        <v>1.06</v>
+        <v>0.82</v>
       </c>
       <c r="K9" s="3">
-        <v>0.68</v>
+        <v>0.27</v>
       </c>
       <c r="L9" s="3">
         <v>0.05</v>
       </c>
+      <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2.65</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.17</v>
+      </c>
       <c r="E10" s="3"/>
-      <c r="F10" s="3">
-        <v>0.89</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0.22</v>
-      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3">
-        <v>0.05</v>
+        <v>0.17</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3">
-        <v>0.93</v>
-      </c>
+      <c r="J10" s="3"/>
       <c r="K10" s="3">
-        <v>0.48</v>
+        <v>0</v>
       </c>
       <c r="L10" s="3">
-        <v>0.05</v>
-      </c>
+        <v>0.17</v>
+      </c>
+      <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3">
-        <v>2.65</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="C11" s="3">
-        <v>0.63</v>
+        <v>0.37</v>
       </c>
       <c r="D11" s="3">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
       <c r="L11" s="3">
-        <v>0.17</v>
-      </c>
+        <v>0.2</v>
+      </c>
+      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
-        <v>1.1299999999999999</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="D12" s="3">
-        <v>0.2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.35</v>
+      </c>
       <c r="H12" s="3">
-        <v>0.2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="J12" s="3">
+        <v>0.93</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.35</v>
+      </c>
       <c r="L12" s="3">
-        <v>0.2</v>
-      </c>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
-        <v>1</v>
+        <v>1.32</v>
       </c>
       <c r="C13" s="3">
-        <v>0.27</v>
+        <v>0.54</v>
       </c>
       <c r="D13" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="3">
-        <v>1.02</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.32</v>
-      </c>
-      <c r="H13" s="3">
-        <v>7.0000000000000007E-2</v>
+      <c r="F13" s="9">
+        <v>1.01</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0.65</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0.1</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3">
-        <v>1.02</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0.61</v>
-      </c>
-      <c r="L13" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="J13" s="9">
+        <v>1.01</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0.35</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
       <c r="P13" s="3"/>
-      <c r="R13" s="3"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3">
-        <v>1.32</v>
+        <v>0.81</v>
       </c>
       <c r="C14" s="3">
-        <v>0.54</v>
+        <v>0.47</v>
       </c>
       <c r="D14" s="3">
         <v>0.1</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="9">
-        <v>1.21</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0.52</v>
-      </c>
-      <c r="H14" s="9">
-        <v>0.1</v>
-      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="9">
-        <v>1.21</v>
-      </c>
-      <c r="K14" s="9">
-        <v>1.04</v>
-      </c>
-      <c r="L14" s="9">
-        <v>0.1</v>
-      </c>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="R14" s="3"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="J14" s="10"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3">
-        <v>0.81</v>
+        <v>1.25</v>
       </c>
       <c r="C15" s="3">
-        <v>0.47</v>
+        <v>0.48</v>
       </c>
       <c r="D15" s="3">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="R15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3">
-        <v>1.25</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.48</v>
-      </c>
-      <c r="D16" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="J15" s="3">
+        <v>1</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.495</v>
+      </c>
+      <c r="L15" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="G16" s="3">
-        <f>0.75/2</f>
-        <v>0.375</v>
-      </c>
-      <c r="H16" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="L16" s="3">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="R16" s="3"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Validation: updated the summary spreadsheet of V&V comparisons
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -578,7 +578,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -658,10 +658,10 @@
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="G3" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="H3" s="3">
         <v>7.0000000000000007E-2</v>

</xml_diff>

<commit_message>
cfast source: removed unused variable NEUTRAL from CFAST data common block
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="4260" windowWidth="25605" windowHeight="18765" tabRatio="500"/>
+    <workbookView xWindow="8955" yWindow="4260" windowWidth="25605" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="J1" sqref="J1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -668,10 +668,11 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3">
-        <v>1.1200000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="K3" s="3">
-        <v>0.215</v>
+        <f>0.44/2</f>
+        <v>0.22</v>
       </c>
       <c r="L3" s="3">
         <v>7.0000000000000007E-2</v>
@@ -705,10 +706,11 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3">
-        <v>1.04</v>
+        <v>1.01</v>
       </c>
       <c r="K4" s="3">
-        <v>0.15</v>
+        <f>0.32/2</f>
+        <v>0.16</v>
       </c>
       <c r="L4" s="3">
         <v>7.0000000000000007E-2</v>
@@ -742,10 +744,11 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3">
-        <v>1.19</v>
+        <v>1.25</v>
       </c>
       <c r="K5" s="3">
-        <v>0.18</v>
+        <f>0.53/2</f>
+        <v>0.26500000000000001</v>
       </c>
       <c r="L5" s="3">
         <v>0.05</v>
@@ -783,7 +786,8 @@
         <v>1.17</v>
       </c>
       <c r="K6" s="3">
-        <v>0.215</v>
+        <f>0.42/2</f>
+        <v>0.21</v>
       </c>
       <c r="L6" s="3">
         <v>7.0000000000000007E-2</v>
@@ -836,10 +840,11 @@
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3">
-        <v>0.97</v>
+        <v>1.03</v>
       </c>
       <c r="K8" s="3">
-        <v>0.32</v>
+        <f>0.63/2</f>
+        <v>0.315</v>
       </c>
       <c r="L8" s="3">
         <v>0.05</v>
@@ -870,7 +875,8 @@
         <v>0.82</v>
       </c>
       <c r="K9" s="3">
-        <v>0.27</v>
+        <f>0.56/2</f>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L9" s="3">
         <v>0.05</v>
@@ -900,9 +906,7 @@
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3">
-        <v>0</v>
-      </c>
+      <c r="K10" s="3"/>
       <c r="L10" s="3">
         <v>0.17</v>
       </c>
@@ -931,9 +935,7 @@
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3">
-        <v>0</v>
-      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="3">
         <v>0.2</v>
       </c>
@@ -1006,7 +1008,8 @@
         <v>1.01</v>
       </c>
       <c r="K13" s="9">
-        <v>0.35</v>
+        <f>1.29/2</f>
+        <v>0.64500000000000002</v>
       </c>
       <c r="L13" s="9">
         <v>0.1</v>
@@ -1065,9 +1068,10 @@
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="K15" s="3">
+        <f>0.99/2</f>
         <v>0.495</v>
       </c>
       <c r="L15" s="3">

</xml_diff>

<commit_message>
Validation: Updated validation scripts to udpate Dunes 200 and ATF tests
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Output Quantity</t>
   </si>
@@ -72,13 +72,19 @@
     <t>Wall Temperature Rise</t>
   </si>
   <si>
-    <t>NUREG-1934</t>
-  </si>
-  <si>
-    <t>RP, 1824 only (new McT algorithm)</t>
-  </si>
-  <si>
-    <t>RP all  (new McT algorithm)</t>
+    <t>Smoke Alarm Activation Time</t>
+  </si>
+  <si>
+    <t>Sprinkler Activation Time</t>
+  </si>
+  <si>
+    <t>RP, 1824 only</t>
+  </si>
+  <si>
+    <t>RP all</t>
+  </si>
+  <si>
+    <t>Original from NUREG-1934</t>
   </si>
 </sst>
 </file>
@@ -173,7 +179,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -202,6 +208,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -575,15 +587,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -591,22 +604,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="1"/>
       <c r="F1" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="J1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
@@ -631,13 +644,13 @@
         <v>3</v>
       </c>
       <c r="I2" s="2"/>
-      <c r="J2" t="s">
+      <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="4"/>
@@ -706,11 +719,11 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3">
-        <v>1.01</v>
+        <v>0.98</v>
       </c>
       <c r="K4" s="3">
-        <f>0.32/2</f>
-        <v>0.16</v>
+        <f>0.45/2</f>
+        <v>0.22500000000000001</v>
       </c>
       <c r="L4" s="3">
         <v>7.0000000000000007E-2</v>
@@ -744,11 +757,11 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3">
-        <v>1.25</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="K5" s="3">
-        <f>0.53/2</f>
-        <v>0.26500000000000001</v>
+        <f>0.43/2</f>
+        <v>0.215</v>
       </c>
       <c r="L5" s="3">
         <v>0.05</v>
@@ -808,9 +821,6 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="P7" s="3"/>
@@ -905,8 +915,6 @@
         <v>0.17</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
       <c r="L10" s="3">
         <v>0.17</v>
       </c>
@@ -934,8 +942,6 @@
         <v>0.2</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
       <c r="L11" s="3">
         <v>0.2</v>
       </c>
@@ -1036,9 +1042,9 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="10"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-      <c r="L14" s="10"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="P14" s="3"/>
@@ -1068,7 +1074,7 @@
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="K15" s="3">
         <f>0.99/2</f>
@@ -1082,6 +1088,9 @@
       <c r="P15" s="3"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1090,9 +1099,33 @@
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="J16" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="K16" s="3">
+        <f>0.98/2</f>
+        <v>0.49</v>
+      </c>
+      <c r="L16" s="3">
+        <f>0.33/2</f>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="K17" s="3">
+        <f>0.52/2</f>
+        <v>0.26</v>
+      </c>
+      <c r="L17" s="3">
+        <f>0.2/2</f>
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
CFAST source: Code cleanup to improve compliance with Fortran 2003.  No change in results verified with full validation suite.
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -200,6 +200,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -208,12 +214,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -590,7 +590,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -603,23 +603,23 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
     </row>
@@ -647,10 +647,10 @@
       <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="M2" s="4"/>
@@ -681,7 +681,7 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3">
-        <v>1.1100000000000001</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K3" s="3">
         <f>0.44/2</f>
@@ -1000,24 +1000,24 @@
         <v>0.1</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="9">
+      <c r="F13" s="11">
         <v>1.01</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="11">
         <v>0.65</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="11">
         <v>0.1</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="9">
+      <c r="J13" s="11">
         <v>1.01</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="11">
         <f>1.29/2</f>
         <v>0.64500000000000002</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="11">
         <v>0.1</v>
       </c>
       <c r="M13" s="5"/>
@@ -1038,13 +1038,13 @@
         <v>0.1</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="3"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="P14" s="3"/>

</xml_diff>

<commit_message>
Validation, Documentation: Updated script and values for validation summary to latest collection of tests.
Editorial corrections to guides.
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -590,7 +590,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3">
-        <v>1.01</v>
+        <v>100</v>
       </c>
       <c r="G4" s="3">
         <v>0.15</v>

</xml_diff>

<commit_message>
Validation: corrected error in runall.bat.  Updated values in V&V comparisons
</commit_message>
<xml_diff>
--- a/cfast/trunk/Validation/VandV Comparison.xlsx
+++ b/cfast/trunk/Validation/VandV Comparison.xlsx
@@ -590,7 +590,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -681,11 +681,11 @@
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3">
-        <v>1.1000000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="K3" s="3">
-        <f>0.44/2</f>
-        <v>0.22</v>
+        <f>0.48/2</f>
+        <v>0.24</v>
       </c>
       <c r="L3" s="3">
         <v>7.0000000000000007E-2</v>
@@ -757,7 +757,7 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3">
-        <v>1.1599999999999999</v>
+        <v>1.23</v>
       </c>
       <c r="K5" s="3">
         <f>0.43/2</f>
@@ -850,11 +850,11 @@
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="K8" s="3">
-        <f>0.63/2</f>
-        <v>0.315</v>
+        <f>0.61/2</f>
+        <v>0.30499999999999999</v>
       </c>
       <c r="L8" s="3">
         <v>0.05</v>
@@ -882,11 +882,11 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3">
-        <v>0.82</v>
+        <v>0.85</v>
       </c>
       <c r="K9" s="3">
-        <f>0.56/2</f>
-        <v>0.28000000000000003</v>
+        <f>0.49/2</f>
+        <v>0.245</v>
       </c>
       <c r="L9" s="3">
         <v>0.05</v>
@@ -1074,11 +1074,11 @@
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3">
-        <v>1</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="K15" s="3">
-        <f>0.99/2</f>
-        <v>0.495</v>
+        <f>0.93/2</f>
+        <v>0.46500000000000002</v>
       </c>
       <c r="L15" s="3">
         <v>7.0000000000000007E-2</v>

</xml_diff>